<commit_message>
acho que esse é o final
</commit_message>
<xml_diff>
--- a/paratecoma-gbif.xlsx
+++ b/paratecoma-gbif.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,6 +413,11 @@
           <t>locality</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>organismID</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1812,6 +1817,11 @@
           <t>Mello Barreto</t>
         </is>
       </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>3736349</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1860,6 +1870,11 @@
           <t>J. G. Kuhlmann</t>
         </is>
       </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>323929</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1908,11 +1923,16 @@
           <t>H. N. Whitford &amp; F. Silveira</t>
         </is>
       </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>271507</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Paratecoma peroba (Record) Kuhlm.</t>
+          <t>Tecoma peroba Record</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1921,14 +1941,14 @@
         </is>
       </c>
       <c r="C32">
-        <v>-19.866667</v>
+        <v>-10.8339</v>
       </c>
       <c r="D32">
-        <v>-40.533333</v>
+        <v>-52.8731</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>gass84,inmano</t>
+          <t>gass84,ambcol,inmafu</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1943,17 +1963,22 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>BOTUw - Xiloteca "Profa. Dra. Maria Aparecida Mourão Brasil"</t>
+          <t>The Field Museum of Natural History</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>BOTUw - Xiloteca "Profa. Dra. Maria Aparecida Mourão Brasil"</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>Comp. Vale do Rio Doce</t>
+          <t>vTypes</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>H. N. Whitford &amp; F. Silveira</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>271506</t>
         </is>
       </c>
     </row>
@@ -1969,37 +1994,85 @@
         </is>
       </c>
       <c r="C33">
+        <v>-19.866667</v>
+      </c>
+      <c r="D33">
+        <v>-40.533333</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>gass84,inmano</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>PRESERVED_SPECIMEN</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>BOTUw - Xiloteca "Profa. Dra. Maria Aparecida Mourão Brasil"</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>BOTUw - Xiloteca "Profa. Dra. Maria Aparecida Mourão Brasil"</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Comp. Vale do Rio Doce</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Paratecoma peroba (Record) Kuhlm.</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Paratecoma peroba (Record) Kuhlm.</t>
+        </is>
+      </c>
+      <c r="C34">
         <v>-21.554722</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>-41.204167</v>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>cdround,gass84,inmano</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>PRESERVED_SPECIMEN</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>PRESERVED_SPECIMEN</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>HUENF</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>Nascimento, M.T.</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>Mata do Funil</t>
         </is>

</xml_diff>